<commit_message>
modified:   Survey.ipynb 	modified:   survey_DB.xlsx
</commit_message>
<xml_diff>
--- a/survey_DB.xlsx
+++ b/survey_DB.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anoban\Documents\Survey_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anoban\Documents\Survey-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB97DFF-6ECF-4A6B-8D47-1E09C2B48539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D5CF6B-AE08-42C6-AA36-E11D6314C0F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22080" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,14 +19,6 @@
     <sheet name="Sheet2" sheetId="6" r:id="rId4"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId5"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">survey!$BI$82:$BJ$82</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">survey!$BK$1:$BK$81</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">survey!$BK$82</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">survey!$BI$82:$BJ$82</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">survey!$BK$1:$BK$81</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">survey!$BK$82</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId6"/>

</xml_diff>